<commit_message>
crawler class and mail_sender methods created
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,58 +434,42 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>title</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>discounted_price</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>main_image_url</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>image_urls</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>rating_score</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>review_count</t>
-        </is>
-      </c>
+      <c r="A1" t="inlineStr"/>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr"/>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>https://cdn.dsmcdn.com/mnresize/420/620/ty608/product/media/images/20221122/13/219567969/629009917/2/2_org_zoom.jpg</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>['https://cdn.dsmcdn.com/mnresize/420/620/ty608/product/media/images/20221122/13/219567969/629009917/2/2_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty607/product/media/images/20221122/13/219567969/629009917/3/3_org_zoom.jpg']</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr"/>
+      <c r="G1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Tresan Isırgan Otu Dökülme Karşıtı Şampuan Normal Ve Kuru Saçlar Için 300 ml X 2 Adet</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
+          <t>S19 Max 4GB+64 GB Beyaz Cep Telefonu (Reeder Türkiye Garantili)</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>3.049 TL</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://cdn.dsmcdn.com/mnresize/420/620/ty1144/product/media/images/prod/SPM/PIM/20240123/12/2f7910b1-c389-3b6b-a084-eeb15328ae05/1_org_zoom.jpg</t>
+          <t>https://cdn.dsmcdn.com/mnresize/1200/1800/ty844/product/media/images/20230425/13/331879740/844745791/1/1_org_zoom.jpg</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['https://cdn.dsmcdn.com/mnresize/420/620/ty1144/product/media/images/prod/SPM/PIM/20240123/12/2f7910b1-c389-3b6b-a084-eeb15328ae05/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1143/product/media/images/prod/SPM/PIM/20240123/12/169ff689-6526-3f29-b77b-ef1d955062f3/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1143/product/media/images/prod/SPM/PIM/20240123/12/9044fd05-cda1-3213-91a8-f897be62cdd8/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1143/product/media/images/prod/SPM/PIM/20240123/12/0b76a33b-585c-35f6-9bb7-ce181a796b05/1_org_zoom.jpg']</t>
+          <t>['https://cdn.dsmcdn.com/mnresize/1200/1800/ty844/product/media/images/20230425/13/331879740/844745791/1/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/seller-store/resources/hizli-satici.svg', 'https://cdn.dsmcdn.com/seller-store/resources/hizli-satici.svg', 'https://cdn.dsmcdn.com/ty844/product/media/images/20230425/13/331879740/844745791/1/1_org_zoom.jpg']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -494,23 +478,78 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Valiberta Çift Cep Kapaklı Kaşe Gömlek - Lacivert</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
+          <t>S19 Max 4GB+64 GB Mavi Cep Telefonu (Reeder Türkiye Garantili)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2.999 TL</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://cdn.dsmcdn.com/mnresize/420/620/ty1024/product/media/images/prod/SPM/PIM/20231027/17/f98c0806-e4cf-3d3c-9e97-bb653a66ea88/1_org_zoom.jpg</t>
+          <t>https://cdn.dsmcdn.com/mnresize/1200/1800/ty847/product/media/images/20230426/11/332690742/918949896/1/1_org_zoom.jpg</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['https://cdn.dsmcdn.com/mnresize/420/620/ty1024/product/media/images/prod/SPM/PIM/20231027/17/f98c0806-e4cf-3d3c-9e97-bb653a66ea88/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1023/product/media/images/prod/SPM/PIM/20231027/17/3b239549-1423-3676-963b-5512d79cb19d/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1025/product/media/images/prod/SPM/PIM/20231027/17/7f432c31-430b-34d6-9b8f-9ddceb00a5a4/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1025/product/media/images/prod/SPM/PIM/20231027/17/435c779d-c260-3936-ae5c-f713cf6a4f9d/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1024/product/media/images/prod/SPM/PIM/20231027/17/d0faf84a-8aa5-3373-9351-4c8342d90860/1_org_zoom.jpg']</t>
+          <t>['https://cdn.dsmcdn.com/mnresize/1200/1800/ty847/product/media/images/20230426/11/332690742/918949896/1/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/ty847/product/media/images/20230426/11/332690742/918949896/1/1_org_zoom.jpg']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://cdn.dsmcdn.com/mnresize/420/620/ty721/product/media/images/20230206/13/276465872/476930554/2/2_org_zoom.jpg</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>['https://cdn.dsmcdn.com/mnresize/420/620/ty721/product/media/images/20230206/13/276465872/476930554/2/2_org_zoom.jpg']</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://cdn.dsmcdn.com/mnresize/420/620/ty508/product/media/images/20220817/9/161294330/545780249/2/2_org_zoom.jpg</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>['https://cdn.dsmcdn.com/mnresize/420/620/ty508/product/media/images/20220817/9/161294330/545780249/2/2_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty507/product/media/images/20220817/9/161294330/545780249/3/3_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty507/product/media/images/20220817/9/161294330/545780249/4/4_org_zoom.jpg']</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://cdn.dsmcdn.com/mnresize/420/620/ty1150/product/media/images/prod/SPM/PIM/20240128/22/78a625f6-dc3d-3c43-9f55-7bf2c78824bd/1_org_zoom.jpg</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>['https://cdn.dsmcdn.com/mnresize/420/620/ty1150/product/media/images/prod/SPM/PIM/20240128/22/78a625f6-dc3d-3c43-9f55-7bf2c78824bd/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1150/product/media/images/prod/SPM/PIM/20240128/22/93b8d939-c7f8-3225-b0c7-5b619c23490f/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1150/product/media/images/prod/SPM/PIM/20240128/22/a8abc4bf-a44a-3ab6-8da7-b75d0057aecc/1_org_zoom.jpg']</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added rules for sending emails. Updated to get url for N11 and Trendyol.
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -434,21 +434,33 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr"/>
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Caterpillar Colorado Erkek Kahverengi Nubuk Bot-637</t>
+        </is>
+      </c>
       <c r="B1" t="inlineStr"/>
       <c r="C1" t="inlineStr"/>
       <c r="D1" t="inlineStr">
         <is>
-          <t>https://cdn.dsmcdn.com/mnresize/420/620/ty1172/product/media/images/prod/SPM/PIM/20240216/18/9d0b0ba0-889a-376b-b5e7-4637f8085090/1_org_zoom.jpg</t>
+          <t>https://n11scdn.akamaized.net/a1/602_857/13/22/22/80/IMG-4041382771724777596.jpg</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>['https://cdn.dsmcdn.com/mnresize/420/620/ty1172/product/media/images/prod/SPM/PIM/20240216/18/9d0b0ba0-889a-376b-b5e7-4637f8085090/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1171/product/media/images/prod/SPM/PIM/20240216/18/4d76074f-b98f-3e46-8aba-190e7f1f1860/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1171/product/media/images/prod/SPM/PIM/20240216/18/e49b51de-4162-3dc7-b535-fd31c05b2872/1_org_zoom.jpg']</t>
+          <t>['https://n11scdn.akamaized.net/a1/602_857/13/22/22/80/IMG-4041382771724777596.jpg', 'https://n11scdn.akamaized.net/a1/60_86/13/22/22/80/IMG-4041382771724777596.jpg', 'https://n11scdn.akamaized.net/a1/60_86/08/64/63/42/IMG-6424608762558479759.jpg', 'https://n11scdn.akamaized.net/a1/60_86/07/88/62/46/IMG-8736130210984762394.jpg', 'https://n11scdn.akamaized.net/a1/60_86/01/83/99/49/IMG-489356320240617610.jpg', 'https://n11scdn.akamaized.net/a1/60_86/09/61/74/63/IMG-9115817892814919145.jpg', 'https://n11scdn.akamaized.net/a1/500_700/24/01/17/72/20/82/70/41/44/34/40/23/97881136301522895152.png']</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr"/>
-      <c r="G1" t="inlineStr"/>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>4.5</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Sending the collected data in the body of the email with a nicely formatted table
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -425,14 +425,40 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ikisi de değil</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>180 TL</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>290 TL</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr"/>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>['https://cdn.dsmcdn.com/mnresize/1200/1800/ty1157/product/media/images/prod/SPM/PIM/20240202/12/61fa1b61-7552-3f42-9812-6eac2c073ca1/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/ty1157/product/media/images/prod/SPM/PIM/20240202/12/61fa1b61-7552-3f42-9812-6eac2c073ca1/1_org_zoom.jpg']</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr"/>
+      <c r="G1" t="inlineStr"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Critical data was written as validated output.
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,27 +436,81 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ikisi de değil</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>180 TL</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>290 TL</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr"/>
+          <t>Amazfit Active Akıllı Saat (Amazfit Türkiye Garantili)</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr"/>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>https://n11scdn.akamaized.net/a1/602_857/09/67/05/91/IMG-1977890781065674594.jpg</t>
+        </is>
+      </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>['https://cdn.dsmcdn.com/mnresize/1200/1800/ty1157/product/media/images/prod/SPM/PIM/20240202/12/61fa1b61-7552-3f42-9812-6eac2c073ca1/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/ty1157/product/media/images/prod/SPM/PIM/20240202/12/61fa1b61-7552-3f42-9812-6eac2c073ca1/1_org_zoom.jpg']</t>
+          <t>['https://n11scdn.akamaized.net/a1/602_857/09/67/05/91/IMG-1977890781065674594.jpg', 'https://n11scdn.akamaized.net/a1/60_86/09/67/05/91/IMG-1977890781065674594.jpg', 'https://n11scdn.akamaized.net/a1/60_86/15/25/87/43/IMG-5803356974882669716.jpg', 'https://n11scdn.akamaized.net/a1/60_86/09/43/32/64/IMG-7912115531430129761.jpg', 'https://n11scdn.akamaized.net/a1/60_86/13/08/46/93/IMG-887897739486994108.jpg', 'https://n11scdn.akamaized.net/a1/60_86/15/37/66/19/IMG-2094926088427494656.jpg', 'https://n11scdn.akamaized.net/a1/60_86/03/40/38/24/IMG-422236255780343523.jpg']</t>
         </is>
       </c>
       <c r="F1" t="inlineStr"/>
       <c r="G1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Samsung Galaxy Tab A9+ Wi-Fi SM-X210 8 GB 128 GB 11" Tablet</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://n11scdn.akamaized.net/a1/602_857/10/00/94/73/IMG-3886570089543208949.jpg</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>['https://n11scdn.akamaized.net/a1/602_857/10/00/94/73/IMG-3886570089543208949.jpg', 'https://n11scdn.akamaized.net/a1/60_86/10/00/94/73/IMG-3886570089543208949.jpg', 'https://n11scdn.akamaized.net/a1/60_86/07/30/60/21/IMG-8525196323097482019.jpg', 'https://n11scdn.akamaized.net/a1/60_86/16/32/70/81/IMG-2575484217061974956.jpg', 'https://n11scdn.akamaized.net/a1/60_86/09/00/03/42/IMG-7057197388026173745.jpg', 'https://n11scdn.akamaized.net/a1/60_86/06/45/35/09/IMG-5919884287401727627.jpg', 'https://n11scdn.akamaized.net/a1/60_86/14/00/73/40/IMG-8217500455611729157.jpg', 'https://n11scdn.akamaized.net/a1/500_700/24/02/16/74/20/86/91/76/06/26/05/54/86651391626104357813.png', 'https://n11scdn.akamaized.net/a1/500_700/24/02/16/62/80/80/79/32/08/78/38/14/92412933804080057162.png', 'https://n11scdn.akamaized.net/a1/500_700/24/02/16/81/07/39/21/28/39/63/27/84/71086975294612718064.png', 'https://n11scdn.akamaized.net/a1/500_700/24/02/09/48/31/90/25/04/04/21/94/49/31917057263205894343.png']</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>4,5</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>67</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Xiaomi Mi Wifi Pro 300 Mbps 2.4 GHz Sinyal Güçlendirici (Türkiye Versiyon)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://n11scdn.akamaized.net/a1/602_857/05/53/69/25/IMG-8811551717331288430.jpg</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>['https://n11scdn.akamaized.net/a1/602_857/05/53/69/25/IMG-8811551717331288430.jpg', 'https://n11scdn.akamaized.net/a1/60_86/05/53/69/25/IMG-8811551717331288430.jpg', 'https://n11scdn.akamaized.net/a1/60_86/07/37/79/79/IMG-2780517974147884701.jpg', 'https://n11scdn.akamaized.net/a1/60_86/02/00/95/36/82946241.jpg', 'https://n11scdn.akamaized.net/a1/60_86/10/67/88/52/IMG-4204343210519024103.jpg', 'https://n11scdn.akamaized.net/a1/60_86/15/31/87/26/IMG-5272898711302070857.jpg', 'https://n11scdn.akamaized.net/a1/500_700/24/02/23/58/97/55/05/84/44/66/61/08/95371355153595515091.jpg', 'https://n11scdn.akamaized.net/a1/500_700/24/02/23/91/42/47/78/15/63/37/13/49/76186264513104557719.jpg', 'https://n11scdn.akamaized.net/a1/500_700/24/02/22/78/47/90/19/93/38/56/20/71/23358246157126711727.png', 'https://n11scdn.akamaized.net/a1/500_700/24/02/22/52/97/97/95/08/50/87/08/46/25891089956506912282.png', 'https://n11scdn.akamaized.net/a1/500_700/24/02/22/92/06/22/49/18/43/74/50/04/36802597043987331134.png']</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>4,5</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>8168</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
some bugs fixed and text rewrited
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,19 +436,23 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Amazfit Active Akıllı Saat (Amazfit Türkiye Garantili)</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr"/>
+          <t>Altınyıldız Classics</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>249,99 TL</t>
+        </is>
+      </c>
       <c r="C1" t="inlineStr"/>
       <c r="D1" t="inlineStr">
         <is>
-          <t>https://n11scdn.akamaized.net/a1/602_857/09/67/05/91/IMG-1977890781065674594.jpg</t>
+          <t>https://cdn.dsmcdn.com/mnresize/420/620/ty80/product/media/images/20210308/18/69852728/137294414/1/1_org_zoom.jpg</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>['https://n11scdn.akamaized.net/a1/602_857/09/67/05/91/IMG-1977890781065674594.jpg', 'https://n11scdn.akamaized.net/a1/60_86/09/67/05/91/IMG-1977890781065674594.jpg', 'https://n11scdn.akamaized.net/a1/60_86/15/25/87/43/IMG-5803356974882669716.jpg', 'https://n11scdn.akamaized.net/a1/60_86/09/43/32/64/IMG-7912115531430129761.jpg', 'https://n11scdn.akamaized.net/a1/60_86/13/08/46/93/IMG-887897739486994108.jpg', 'https://n11scdn.akamaized.net/a1/60_86/15/37/66/19/IMG-2094926088427494656.jpg', 'https://n11scdn.akamaized.net/a1/60_86/03/40/38/24/IMG-422236255780343523.jpg']</t>
+          <t>['https://cdn.dsmcdn.com/mnresize/420/620/ty81/product/media/images/20210308/18/69852728/137294414/2/2_org_zoom.jpg']</t>
         </is>
       </c>
       <c r="F1" t="inlineStr"/>
@@ -457,60 +461,148 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Samsung Galaxy Tab A9+ Wi-Fi SM-X210 8 GB 128 GB 11" Tablet</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr"/>
+          <t>Happiness İstanbul</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>239,48 TL</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://n11scdn.akamaized.net/a1/602_857/10/00/94/73/IMG-3886570089543208949.jpg</t>
+          <t>https://cdn.dsmcdn.com/mnresize/420/620/ty496/product/media/images/20220801/13/153049070/533113392/2/2_org_zoom.jpg</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['https://n11scdn.akamaized.net/a1/602_857/10/00/94/73/IMG-3886570089543208949.jpg', 'https://n11scdn.akamaized.net/a1/60_86/10/00/94/73/IMG-3886570089543208949.jpg', 'https://n11scdn.akamaized.net/a1/60_86/07/30/60/21/IMG-8525196323097482019.jpg', 'https://n11scdn.akamaized.net/a1/60_86/16/32/70/81/IMG-2575484217061974956.jpg', 'https://n11scdn.akamaized.net/a1/60_86/09/00/03/42/IMG-7057197388026173745.jpg', 'https://n11scdn.akamaized.net/a1/60_86/06/45/35/09/IMG-5919884287401727627.jpg', 'https://n11scdn.akamaized.net/a1/60_86/14/00/73/40/IMG-8217500455611729157.jpg', 'https://n11scdn.akamaized.net/a1/500_700/24/02/16/74/20/86/91/76/06/26/05/54/86651391626104357813.png', 'https://n11scdn.akamaized.net/a1/500_700/24/02/16/62/80/80/79/32/08/78/38/14/92412933804080057162.png', 'https://n11scdn.akamaized.net/a1/500_700/24/02/16/81/07/39/21/28/39/63/27/84/71086975294612718064.png', 'https://n11scdn.akamaized.net/a1/500_700/24/02/09/48/31/90/25/04/04/21/94/49/31917057263205894343.png']</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>4,5</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>67</t>
-        </is>
-      </c>
+          <t>['https://cdn.dsmcdn.com/mnresize/420/620/ty497/product/media/images/20220801/13/153049070/533113392/3/3_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty497/product/media/images/20220801/13/153049070/533113392/4/4_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty497/product/media/images/20220801/13/153049070/533113392/5/5_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty495/product/media/images/20220801/13/153049070/533113392/6/6_org_zoom.jpg']</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Xiaomi Mi Wifi Pro 300 Mbps 2.4 GHz Sinyal Güçlendirici (Türkiye Versiyon)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>https://n11scdn.akamaized.net/a1/602_857/05/53/69/25/IMG-8811551717331288430.jpg</t>
-        </is>
-      </c>
+          <t>Default Title</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>163,29 TL</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>165,64 TL</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['https://n11scdn.akamaized.net/a1/602_857/05/53/69/25/IMG-8811551717331288430.jpg', 'https://n11scdn.akamaized.net/a1/60_86/05/53/69/25/IMG-8811551717331288430.jpg', 'https://n11scdn.akamaized.net/a1/60_86/07/37/79/79/IMG-2780517974147884701.jpg', 'https://n11scdn.akamaized.net/a1/60_86/02/00/95/36/82946241.jpg', 'https://n11scdn.akamaized.net/a1/60_86/10/67/88/52/IMG-4204343210519024103.jpg', 'https://n11scdn.akamaized.net/a1/60_86/15/31/87/26/IMG-5272898711302070857.jpg', 'https://n11scdn.akamaized.net/a1/500_700/24/02/23/58/97/55/05/84/44/66/61/08/95371355153595515091.jpg', 'https://n11scdn.akamaized.net/a1/500_700/24/02/23/91/42/47/78/15/63/37/13/49/76186264513104557719.jpg', 'https://n11scdn.akamaized.net/a1/500_700/24/02/22/78/47/90/19/93/38/56/20/71/23358246157126711727.png', 'https://n11scdn.akamaized.net/a1/500_700/24/02/22/52/97/97/95/08/50/87/08/46/25891089956506912282.png', 'https://n11scdn.akamaized.net/a1/500_700/24/02/22/92/06/22/49/18/43/74/50/04/36802597043987331134.png']</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>4,5</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>8168</t>
-        </is>
-      </c>
+          <t>['https://cdn.dsmcdn.com/mnresize/1200/1800/ty1162/product/media/images/prod/SPM/PIM/20240206/15/bf8ceb40-539b-3e2d-9aa0-555191680f22/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/ty1162/product/media/images/prod/SPM/PIM/20240206/15/bf8ceb40-539b-3e2d-9aa0-555191680f22/1_org_zoom.jpg']</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Default Title</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>247,87 TL</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>['https://cdn.dsmcdn.com/mnresize/1200/1800/ty999/product/media/images/prod/PIM/20230918/11/e24750c5-08e8-4457-9e97-07d1bf7a4181/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/ty999/product/media/images/prod/PIM/20230918/11/e24750c5-08e8-4457-9e97-07d1bf7a4181/1_org_zoom.jpg']</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Default Title</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>349 TL</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://cdn.dsmcdn.com/mnresize/420/620/ty1143/product/media/images/prod/SPM/PIM/20240122/19/d6b9e8ea-eadb-3352-b11c-b793f27e5dca/1_org_zoom.jpg</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>['https://cdn.dsmcdn.com/mnresize/420/620/ty1144/product/media/images/prod/SPM/PIM/20240122/19/5ecad0a9-639b-377d-ab88-5e043c1da4bf/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1144/product/media/images/prod/SPM/PIM/20240122/19/182ea6e2-b62a-36e0-8c14-3336328a1bfe/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1144/product/media/images/prod/SPM/PIM/20240122/19/0175491e-2c51-3c1a-a074-7427bc490c03/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1145/product/media/images/prod/SPM/PIM/20240122/19/1f66bb55-7ad0-309e-ba61-24f499f4e7c8/1_org_zoom.jpg']</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Twisted Minds</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1.205 TL</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://cdn.dsmcdn.com/mnresize/420/620/ty1006/product/media/images/prod/SPM/PIM/20230929/09/d5f4cec3-e06c-3ae7-b3d5-d61fbc79db36/1_org_zoom.jpg</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>['https://cdn.dsmcdn.com/mnresize/420/620/ty1005/product/media/images/prod/SPM/PIM/20230929/09/26f15a9e-199c-3f2a-8cce-d071aed38376/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1006/product/media/images/prod/SPM/PIM/20230929/09/82502fea-32ab-35fa-8784-68c79fb5552f/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1006/product/media/images/prod/SPM/PIM/20230929/09/4810b651-27e1-3663-92b2-f966cbe62f48/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/mnresize/420/620/ty1005/product/media/images/prod/SPM/PIM/20230929/09/4312aaf8-ba56-3379-b367-ba3a0950e8bb/1_org_zoom.jpg']</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Default Title</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2.519 TL</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2.919 TL</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>['https://cdn.dsmcdn.com/mnresize/1200/1800/ty1026/product/media/images/prod/SPM/PIM/20231030/13/2e233745-406f-348a-a33f-6086a5d6a8ad/1_org_zoom.jpg', 'https://cdn.dsmcdn.com/ty1026/product/media/images/prod/SPM/PIM/20231030/13/2e233745-406f-348a-a33f-6086a5d6a8ad/1_org_zoom.jpg']</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>